<commit_message>
eadmin report and config
</commit_message>
<xml_diff>
--- a/src/assets/img/DataList.xlsx
+++ b/src/assets/img/DataList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Medha Office\Projects\SIDP-FE-2025\src\assets\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F126170A-A394-4571-B3E4-330CAE094A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8EFE5E-4F20-499B-8BE8-99C7927C8E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9097DA4C-51A9-4AF0-990A-E08C94682FFE}"/>
   </bookViews>
@@ -36,118 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
-  <si>
-    <t>States names</t>
-  </si>
-  <si>
-    <t>Andaman and Nicobar Islands</t>
-  </si>
-  <si>
-    <t>Andhra Pradesh</t>
-  </si>
-  <si>
-    <t>Arunachal Pradesh</t>
-  </si>
-  <si>
-    <t>Assam</t>
-  </si>
-  <si>
-    <t>Bihar</t>
-  </si>
-  <si>
-    <t>Chandigarh</t>
-  </si>
-  <si>
-    <t>Chhattisgarh</t>
-  </si>
-  <si>
-    <t>Dadra and Nagar Haveli and Daman and Diu</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>Gujarat</t>
-  </si>
-  <si>
-    <t>Haryana</t>
-  </si>
-  <si>
-    <t>Himachal Pradesh</t>
-  </si>
-  <si>
-    <t>Jammu and Kashmir</t>
-  </si>
-  <si>
-    <t>Jharkhand</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
-  </si>
-  <si>
-    <t>Kerala</t>
-  </si>
-  <si>
-    <t>Ladakh</t>
-  </si>
-  <si>
-    <t>Lakshadweep</t>
-  </si>
-  <si>
-    <t>Madhya Pradesh</t>
-  </si>
-  <si>
-    <t>Maharashtra</t>
-  </si>
-  <si>
-    <t>Manipur</t>
-  </si>
-  <si>
-    <t>Meghalaya</t>
-  </si>
-  <si>
-    <t>Mizoram</t>
-  </si>
-  <si>
-    <t>Nagaland</t>
-  </si>
-  <si>
-    <t>Odisha</t>
-  </si>
-  <si>
-    <t>Puducherry</t>
-  </si>
-  <si>
-    <t>Punjab</t>
-  </si>
-  <si>
-    <t>Rajasthan</t>
-  </si>
-  <si>
-    <t>Sikkim</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
-    <t>Telangana</t>
-  </si>
-  <si>
-    <t>Tripura</t>
-  </si>
-  <si>
-    <t>Uttar Pradesh</t>
-  </si>
-  <si>
-    <t>Uttarakhand</t>
-  </si>
-  <si>
-    <t>West Bengal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>English</t>
   </si>
@@ -198,6 +87,123 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>District Names</t>
+  </si>
+  <si>
+    <t>ARIYALUR</t>
+  </si>
+  <si>
+    <t>CHENGALPATTU</t>
+  </si>
+  <si>
+    <t>CHENNAI</t>
+  </si>
+  <si>
+    <t>COIMBATORE</t>
+  </si>
+  <si>
+    <t>CUDDALORE</t>
+  </si>
+  <si>
+    <t>DHARMAPURI</t>
+  </si>
+  <si>
+    <t>DINDIGUL</t>
+  </si>
+  <si>
+    <t>ERODE</t>
+  </si>
+  <si>
+    <t>KALLAKURICHI</t>
+  </si>
+  <si>
+    <t>KANCHEEPURAM</t>
+  </si>
+  <si>
+    <t>KANNIYAKUMARI</t>
+  </si>
+  <si>
+    <t>KARUR</t>
+  </si>
+  <si>
+    <t>KRISHNAGIRI</t>
+  </si>
+  <si>
+    <t>MADURAI</t>
+  </si>
+  <si>
+    <t>MAYILADUTHURAI</t>
+  </si>
+  <si>
+    <t>NAGAPATTINAM</t>
+  </si>
+  <si>
+    <t>NAMAKKAL</t>
+  </si>
+  <si>
+    <t>PERAMBALUR</t>
+  </si>
+  <si>
+    <t>PUDUKKOTTAI</t>
+  </si>
+  <si>
+    <t>RAMANATHAPURAM</t>
+  </si>
+  <si>
+    <t>RANIPET</t>
+  </si>
+  <si>
+    <t>SALEM</t>
+  </si>
+  <si>
+    <t>SIVAGANGA</t>
+  </si>
+  <si>
+    <t>TENKASI</t>
+  </si>
+  <si>
+    <t>THANJAVUR</t>
+  </si>
+  <si>
+    <t>THE NILGIRIS</t>
+  </si>
+  <si>
+    <t>THENI</t>
+  </si>
+  <si>
+    <t>THIRUVALLUR</t>
+  </si>
+  <si>
+    <t>THIRUVARUR</t>
+  </si>
+  <si>
+    <t>THOOTHUKKUDI</t>
+  </si>
+  <si>
+    <t>TIRUCHIRAPPALLI</t>
+  </si>
+  <si>
+    <t>TIRUNELVELI</t>
+  </si>
+  <si>
+    <t>TIRUPATHUR</t>
+  </si>
+  <si>
+    <t>TIRUPPUR</t>
+  </si>
+  <si>
+    <t>TIRUVANNAMALAI</t>
+  </si>
+  <si>
+    <t>VELLORE</t>
+  </si>
+  <si>
+    <t>VILUPPURAM</t>
+  </si>
+  <si>
+    <t>VIRUDHUNAGAR</t>
   </si>
 </sst>
 </file>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DC0F86-3C3D-4729-99EA-E212F3ACADC4}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,296 +607,306 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
+      <c r="A10" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
+      <c r="A11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
+      <c r="A12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
+      <c r="A13" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
+      <c r="A14" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
+      <c r="A15" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
+      <c r="A16" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
+      <c r="A17" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
+      <c r="A18" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
+      <c r="A19" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+      <c r="A20" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
+      <c r="A21" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
+      <c r="A22" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
+      <c r="A23" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
+      <c r="A24" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
+      <c r="A25" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
+      <c r="A26" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
+      <c r="A27" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
+      <c r="A28" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
+      <c r="A29" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
+      <c r="A30" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
+      <c r="A31" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
+      <c r="A32" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>32</v>
+      <c r="A33" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>33</v>
+      <c r="A34" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>34</v>
+      <c r="A35" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>